<commit_message>
kapital processed data is perfect
</commit_message>
<xml_diff>
--- a/processed_data/kapital_bank_excel/2020_Q1/capital_adequacy_2020_Q1.xlsx
+++ b/processed_data/kapital_bank_excel/2020_Q1/capital_adequacy_2020_Q1.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,10 +448,8 @@
           <t>Bank kapitalının strukturu və adekvatlığı barədə məlumatlar</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>(min manatla)</t>
@@ -859,7 +858,113 @@
           <t>*risk qruplarının tərkibi "Bank kapitalının və onun adekvatlığının hesablanması Qaydaları" ilə müəyyən</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Əmsal</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Norma (Sistem əhəmiyyətli)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Norma (Banklar istisna)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fakt</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>9.  I dərəcəli  kapitalın  adekvatlıq əmsalı</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01.01.2020-yə qədər</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>minimum 5%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>14.89%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>10. məcmu kapitalın  adekvatlıq  əmsalı</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01.01.2020-yə qədər</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>minimum 10%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>19.14%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>11. Leverec əmsalı</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>minimum 5%</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>minimum 4%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>7.67%</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>